<commit_message>
Implementacion de la funcion agregar al carro de compras
</commit_message>
<xml_diff>
--- a/src/test/resources/data/Data.xlsx
+++ b/src/test/resources/data/Data.xlsx
@@ -24,12 +24,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Producto</t>
   </si>
   <si>
-    <t>nevera</t>
+    <t>Cantidad</t>
+  </si>
+  <si>
+    <t>audifonos</t>
   </si>
 </sst>
 </file>
@@ -80,9 +83,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -363,7 +367,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -371,14 +375,20 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="B2" s="2">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>